<commit_message>
guess I didn't hit save...
</commit_message>
<xml_diff>
--- a/check sample work/christians samples 2021/TA/Christians TA samples compiled 2021.xlsx
+++ b/check sample work/christians samples 2021/TA/Christians TA samples compiled 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rye-Tech\Documents\R\rye-tech-home\2021-season-summary\check sample work\christians samples 2021\TA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5C31A4-1BA6-4851-810B-41818613DE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A76E0D-9D16-4DC3-9D8C-4617368EAA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11160" xr2:uid="{2A57CFC7-A3BC-4562-B084-879118DEC932}"/>
   </bookViews>
@@ -724,7 +724,7 @@
   <dimension ref="A1:M87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
@@ -2428,7 +2428,7 @@
       <c r="L68" s="14"/>
       <c r="M68" s="14"/>
     </row>
-    <row r="69" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A69" s="14" t="s">
         <v>47</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>2322.9161702439701</v>
       </c>
     </row>
-    <row r="73" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="9" t="s">
         <v>58</v>
       </c>

</xml_diff>